<commit_message>
How Paul Saved His GPA-How Steve Jobs Saved Apple
</commit_message>
<xml_diff>
--- a/assignments/cw2 drafts/task-plan.xlsx
+++ b/assignments/cw2 drafts/task-plan.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pcowe/Desktop/python-data-programming/assignments/cw2 drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E33BE60-EFB7-3D41-AE90-D557C3B5DF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2696623-457F-7A4C-846C-93FA459E286F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="480" windowWidth="23160" windowHeight="17540" xr2:uid="{5A9C4F78-ACD2-2E4A-BE11-E176A0F20257}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22760" windowHeight="17540" xr2:uid="{5A9C4F78-ACD2-2E4A-BE11-E176A0F20257}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Task Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Preprocessing" sheetId="2" r:id="rId2"/>
+    <sheet name="Analysis" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
   <si>
     <t>Task</t>
   </si>
@@ -133,14 +136,144 @@
 1.2 Acquire Intellectual Property Filing Data from BigQuery Datawarehouse</t>
   </si>
   <si>
-    <t>2. Data Preprocessing</t>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>Preprocessing Classification</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Referenced Scenario</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Google Trends</t>
+  </si>
+  <si>
+    <t>Google Patents</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Source Table</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>Platforms</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>yearly</t>
+  </si>
+  <si>
+    <t>blockchain</t>
+  </si>
+  <si>
+    <t>youtube</t>
+  </si>
+  <si>
+    <t>web search</t>
+  </si>
+  <si>
+    <t>africa</t>
+  </si>
+  <si>
+    <t>northamerica</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>over many years</t>
+  </si>
+  <si>
+    <t>monthky</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>time class</t>
+  </si>
+  <si>
+    <t>Time granularity</t>
+  </si>
+  <si>
+    <t>each day of the month of december</t>
+  </si>
+  <si>
+    <t>web</t>
+  </si>
+  <si>
+    <t>topics</t>
+  </si>
+  <si>
+    <t>afric</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>each month oct 17 to feb. 18</t>
+  </si>
+  <si>
+    <t>yly</t>
+  </si>
+  <si>
+    <t>7 n 8</t>
+  </si>
+  <si>
+    <t>nft, block, crypto</t>
+  </si>
+  <si>
+    <t>yt</t>
+  </si>
+  <si>
+    <t>2. Data Preprocessing
+2.1 Data Cleaning (Trends)
+2.2 Data Transformation (IP transform to NLP compatible models)
+2.3 Data integration (Trends countries)
+2.4 Data Reduction (sampling patent data)</t>
+  </si>
+  <si>
+    <t>Pattern Extraction</t>
+  </si>
+  <si>
+    <t>Pattern Evaluation</t>
+  </si>
+  <si>
+    <t>Pattern Presentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,13 +304,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -192,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -215,6 +373,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544FAF85-B879-4F49-BD07-4A37D780F047}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -571,7 +738,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="200" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -587,7 +754,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="100" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="220" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -599,8 +766,8 @@
       <c r="E3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>28</v>
+      <c r="G3" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="100" x14ac:dyDescent="0.25">
@@ -614,6 +781,9 @@
       <c r="D4" s="6"/>
       <c r="E4" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="100" x14ac:dyDescent="0.25">
@@ -626,6 +796,9 @@
       <c r="E5" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="G5" s="9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
@@ -636,6 +809,9 @@
       <c r="D6" s="6"/>
       <c r="E6" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.25">
@@ -690,4 +866,469 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7AE063-E37E-3543-97F7-23A9D46243B7}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17ED1A8-98DC-7D4A-A2EC-3D9DFC1C35DE}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A429EF8-7D0E-F84F-A22A-1F9BBBD98FBC}">
+  <dimension ref="A1:P35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N6" s="15"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I15" s="15"/>
+      <c r="P15" s="15"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>